<commit_message>
mostly finalized B2 design
</commit_message>
<xml_diff>
--- a/bom/BOM-B1A.xlsx
+++ b/bom/BOM-B1A.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmeliza/Devel/starboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmeliza/Devel/starboard/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BE4304-0ECE-5B42-A7A3-DA315448C94E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CE875C-861D-4840-BB4B-C16E2898F088}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31160" yWindow="860" windowWidth="28800" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Revised BOM - May 2017" sheetId="1" r:id="rId1"/>
+    <sheet name="Rev B2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="171">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="164">
   <si>
     <t>Reference</t>
   </si>
@@ -103,9 +100,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>C2,C3,C8,C10</t>
-  </si>
-  <si>
     <t>C4,C5</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t>1x5 - 3.5 mm screw terminal</t>
   </si>
   <si>
-    <t>OUT-TTL-IN</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -409,21 +400,6 @@
     <t>https://www.mouser.com/ProductDetail/Phoenix-Contact/1985807/</t>
   </si>
   <si>
-    <t>1x3 pin strip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSW-103-07-L-S </t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200-TSW10307LS </t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samtec/TSW-103-07-L-S</t>
-  </si>
-  <si>
     <t xml:space="preserve">512-FDT439N </t>
   </si>
   <si>
@@ -466,12 +442,6 @@
     <t xml:space="preserve">774-2192LPST </t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Header shunt</t>
-  </si>
-  <si>
     <t>adafruit</t>
   </si>
   <si>
@@ -517,15 +487,6 @@
     <t xml:space="preserve">490-PJ-050BH </t>
   </si>
   <si>
-    <t xml:space="preserve">1-382811-8 </t>
-  </si>
-  <si>
-    <t>TE Connectivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">571-1-382811-8 </t>
-  </si>
-  <si>
     <t>Grand Total</t>
   </si>
   <si>
@@ -533,13 +494,31 @@
   </si>
   <si>
     <t xml:space="preserve">810-C3225X5R1E106K </t>
+  </si>
+  <si>
+    <t>C2,C3,C8,C10,C11,C12,C14</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>CAPACITOR CERAMIC 10UF 6.3V 0603 X5R 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1608X5R0J106K080AB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">810-C1608X5R0J106K </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TDK/C1608X5R0J106K080AB?qs=NRhsANhppD9O7AAk61oBsw%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -567,12 +546,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -653,9 +626,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -690,7 +663,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -728,14 +700,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1019,72 +991,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH91"/>
+  <dimension ref="A1:AG90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23" style="24" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="24" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="24" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="24" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="24" customWidth="1"/>
-    <col min="10" max="11" width="9.1640625" style="24" customWidth="1"/>
-    <col min="12" max="13" width="10" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="23" style="23" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="23" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="23" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="23" customWidth="1"/>
+    <col min="9" max="10" width="9.1640625" style="23" customWidth="1"/>
+    <col min="11" max="12" width="10" style="23" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -1104,52 +1073,49 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-    </row>
-    <row r="2" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8">
+    </row>
+    <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>170</v>
-      </c>
       <c r="I2" s="8">
-        <v>1</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J2" s="8">
+        <f t="shared" ref="J2:J31" si="0">H2*I2</f>
         <v>0.30399999999999999</v>
       </c>
       <c r="K2" s="8">
-        <f t="shared" ref="K2:K72" si="0">I2*J2</f>
-        <v>0.30399999999999999</v>
+        <f>H2*$D$80</f>
+        <v>10</v>
       </c>
       <c r="L2" s="8">
-        <f t="shared" ref="L2:L8" si="1">I2*$E$81</f>
-        <v>10</v>
-      </c>
-      <c r="M2" s="8">
-        <f t="shared" ref="M2:M72" si="2">J2*L2</f>
+        <f t="shared" ref="L2:L31" si="1">I2*K2</f>
         <v>3.04</v>
       </c>
-      <c r="N2" s="26" t="s">
-        <v>122</v>
-      </c>
+      <c r="M2" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1169,52 +1135,49 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="16" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>105</v>
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="8">
+        <v>7</v>
       </c>
       <c r="I3" s="8">
-        <v>4</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="J3" s="8">
-        <v>4.3999999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.308</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" si="0"/>
-        <v>0.17599999999999999</v>
+        <f>H3*$D$80</f>
+        <v>70</v>
       </c>
       <c r="L3" s="8">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="M3" s="8">
-        <f t="shared" si="2"/>
-        <v>1.7599999999999998</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>121</v>
-      </c>
+        <v>3.0799999999999996</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1234,52 +1197,49 @@
       <c r="AE3" s="6"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>107</v>
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2</v>
       </c>
       <c r="I4" s="8">
-        <v>2</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="J4" s="8">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="K4" s="8">
         <f t="shared" si="0"/>
         <v>0.98599999999999999</v>
       </c>
+      <c r="K4" s="8">
+        <f>H4*$D$80</f>
+        <v>20</v>
+      </c>
       <c r="L4" s="8">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="M4" s="8">
-        <f t="shared" si="2"/>
         <v>9.86</v>
       </c>
-      <c r="N4" s="26" t="s">
-        <v>120</v>
-      </c>
+      <c r="M4" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -1299,52 +1259,49 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="8">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>109</v>
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
       </c>
       <c r="I5" s="8">
-        <v>1</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="J5" s="8">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="K5" s="8">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-2</v>
       </c>
+      <c r="K5" s="8">
+        <f>H5*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L5" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="M5" s="8">
-        <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="N5" s="26" t="s">
-        <v>119</v>
-      </c>
+      <c r="M5" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1364,52 +1321,49 @@
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8">
-        <v>5</v>
+    </row>
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
+      <c r="G6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
       </c>
       <c r="I6" s="8">
-        <v>1</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="J6" s="8">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="K6" s="8">
         <f t="shared" si="0"/>
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="K6" s="8">
+        <f>H6*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L6" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="M6" s="8">
-        <f t="shared" si="2"/>
         <v>0.34</v>
       </c>
-      <c r="N6" s="26" t="s">
-        <v>118</v>
-      </c>
+      <c r="M6" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1429,52 +1383,49 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
-      <c r="AH6" s="6"/>
-    </row>
-    <row r="7" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="8">
-        <v>6</v>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>113</v>
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
       </c>
       <c r="I7" s="8">
-        <v>1</v>
+        <v>0.185</v>
       </c>
       <c r="J7" s="8">
-        <v>0.185</v>
-      </c>
-      <c r="K7" s="8">
         <f t="shared" si="0"/>
         <v>0.185</v>
       </c>
+      <c r="K7" s="8">
+        <f>H7*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L7" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="M7" s="8">
-        <f t="shared" si="2"/>
         <v>1.85</v>
       </c>
-      <c r="N7" s="26" t="s">
-        <v>117</v>
-      </c>
+      <c r="M7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1494,117 +1445,111 @@
       <c r="AE7" s="6"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-    </row>
-    <row r="8" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8">
-        <v>7</v>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="25" t="s">
-        <v>103</v>
+        <v>160</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>104</v>
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
       </c>
       <c r="I8" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="K8" s="8">
+        <f>H8*$D$80</f>
+        <v>10</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+    </row>
+    <row r="9" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="8">
         <v>4</v>
       </c>
-      <c r="J8" s="8">
+      <c r="I9" s="8">
         <v>4.1399999999999997</v>
       </c>
-      <c r="K8" s="8">
+      <c r="J9" s="8">
         <f t="shared" si="0"/>
         <v>16.559999999999999</v>
       </c>
-      <c r="L8" s="8">
+      <c r="K9" s="8">
+        <f>H9*$D$80</f>
+        <v>40</v>
+      </c>
+      <c r="L9" s="8">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="M8" s="8">
-        <f t="shared" si="2"/>
         <v>165.6</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-    </row>
-    <row r="9" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>114</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" si="0"/>
-        <v>0.875</v>
-      </c>
-      <c r="L9" s="8">
-        <f t="shared" ref="L9:L72" si="3">I9*$E$81</f>
-        <v>10</v>
-      </c>
-      <c r="M9" s="8">
-        <f t="shared" si="2"/>
-        <v>8.75</v>
-      </c>
-      <c r="N9" s="26" t="s">
-        <v>116</v>
-      </c>
+      <c r="M9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -1624,52 +1569,49 @@
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="6"/>
-      <c r="AH9" s="6"/>
-    </row>
-    <row r="10" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8">
-        <v>9</v>
+    </row>
+    <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>123</v>
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
       </c>
       <c r="I10" s="8">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="J10" s="8">
-        <v>0.28499999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.875</v>
       </c>
       <c r="K10" s="8">
-        <f t="shared" si="0"/>
-        <v>0.28499999999999998</v>
+        <f>H10*$D$80</f>
+        <v>10</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M10" s="8">
-        <f t="shared" si="2"/>
-        <v>2.8499999999999996</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>124</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -1689,52 +1631,49 @@
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-    </row>
-    <row r="11" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8">
+    </row>
+    <row r="11" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K11" s="8">
+        <f>H11*$D$80</f>
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="16">
-        <v>1985807</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" s="8">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="K11" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1399999999999999</v>
-      </c>
       <c r="L11" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M11" s="8">
-        <f t="shared" si="2"/>
-        <v>11.399999999999999</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>128</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -1754,52 +1693,49 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
-    </row>
-    <row r="12" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8">
-        <v>11</v>
+    </row>
+    <row r="12" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="16">
-        <v>1800016</v>
+        <v>35</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="15">
+        <v>1985807</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>126</v>
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
       </c>
       <c r="I12" s="8">
-        <v>1</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="J12" s="8">
-        <v>2.92</v>
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" si="0"/>
-        <v>2.92</v>
+        <f>H12*$D$80</f>
+        <v>10</v>
       </c>
       <c r="L12" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M12" s="8">
-        <f t="shared" si="2"/>
-        <v>29.2</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>127</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>11.399999999999999</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1819,52 +1755,49 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-    </row>
-    <row r="13" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8">
-        <v>12</v>
+    </row>
+    <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="16" t="s">
-        <v>130</v>
+        <v>37</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="15">
+        <v>1800016</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>132</v>
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
       </c>
       <c r="I13" s="8">
-        <v>1</v>
+        <v>2.92</v>
       </c>
       <c r="J13" s="8">
-        <v>0.24299999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.92</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.24299999999999999</v>
+        <f>H13*$D$80</f>
+        <v>10</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M13" s="8">
-        <f t="shared" si="2"/>
-        <v>2.4299999999999997</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>133</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>29.2</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -1884,52 +1817,49 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-    </row>
-    <row r="14" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
-        <v>13</v>
+    </row>
+    <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" t="s">
-        <v>134</v>
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
       </c>
       <c r="I14" s="8">
-        <v>1</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="J14" s="8">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="K14" s="8">
         <f t="shared" si="0"/>
         <v>0.57599999999999996</v>
       </c>
+      <c r="K14" s="8">
+        <f>H14*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L14" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.76</v>
       </c>
-      <c r="N14" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="M14" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -1949,52 +1879,49 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-    </row>
-    <row r="15" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
-        <v>14</v>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>136</v>
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
       </c>
       <c r="I15" s="8">
-        <v>1</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="J15" s="8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K15" s="8">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="K15" s="8">
+        <f>H15*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L15" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="N15" s="26" t="s">
-        <v>137</v>
-      </c>
+      <c r="M15" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2014,50 +1941,47 @@
       <c r="AE15" s="6"/>
       <c r="AF15" s="6"/>
       <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-    </row>
-    <row r="16" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8">
+    </row>
+    <row r="16" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>138</v>
+      <c r="G16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
       </c>
       <c r="I16" s="8">
-        <v>1</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J16" s="8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K16" s="8">
         <f t="shared" si="0"/>
         <v>3.5000000000000003E-2</v>
       </c>
+      <c r="K16" s="8">
+        <f>H16*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L16" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.35000000000000003</v>
       </c>
-      <c r="N16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -2077,50 +2001,47 @@
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-    </row>
-    <row r="17" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8">
-        <v>16</v>
+    </row>
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="16" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="s">
-        <v>136</v>
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
       </c>
       <c r="I17" s="8">
-        <v>1</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="J17" s="8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K17" s="8">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="K17" s="8">
+        <f>H17*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L17" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="N17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
@@ -2140,50 +2061,47 @@
       <c r="AE17" s="6"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
-      <c r="AH17" s="6"/>
-    </row>
-    <row r="18" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="8">
-        <v>17</v>
+    </row>
+    <row r="18" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="16" t="s">
-        <v>99</v>
+        <v>43</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" t="s">
-        <v>139</v>
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
       </c>
       <c r="I18" s="8">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="J18" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="K18" s="8">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
+      <c r="K18" s="8">
+        <f>H18*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L18" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M18" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="N18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
@@ -2203,52 +2121,49 @@
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
-      <c r="AH18" s="6"/>
-    </row>
-    <row r="19" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8">
-        <v>18</v>
+    </row>
+    <row r="19" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" t="s">
-        <v>141</v>
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
       </c>
       <c r="I19" s="8">
-        <v>1</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="J19" s="8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K19" s="8">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="K19" s="8">
+        <f>H19*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L19" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="N19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -2268,50 +2183,47 @@
       <c r="AE19" s="6"/>
       <c r="AF19" s="6"/>
       <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-    </row>
-    <row r="20" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8">
-        <v>19</v>
+    </row>
+    <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="23" t="s">
-        <v>101</v>
+        <v>47</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>142</v>
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
       </c>
       <c r="I20" s="8">
-        <v>1</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="J20" s="8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K20" s="8">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="K20" s="8">
+        <f>H20*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L20" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M20" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="N20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -2331,50 +2243,47 @@
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="6"/>
-      <c r="AH20" s="6"/>
-    </row>
-    <row r="21" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="8">
-        <v>20</v>
+    </row>
+    <row r="21" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="16" t="s">
-        <v>143</v>
+        <v>49</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s">
-        <v>144</v>
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="8">
+        <v>2</v>
       </c>
       <c r="I21" s="8">
-        <v>2</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="J21" s="8">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="K21" s="8">
         <f t="shared" si="0"/>
         <v>0.28799999999999998</v>
       </c>
+      <c r="K21" s="8">
+        <f>H21*$D$80</f>
+        <v>20</v>
+      </c>
       <c r="L21" s="8">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="M21" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
-      <c r="N21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -2394,50 +2303,47 @@
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-    </row>
-    <row r="22" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8">
-        <v>21</v>
+    </row>
+    <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="11" t="s">
-        <v>102</v>
+        <v>51</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" t="s">
-        <v>145</v>
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1</v>
       </c>
       <c r="I22" s="8">
-        <v>1</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="J22" s="8">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K22" s="8">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="K22" s="8">
+        <f>H22*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L22" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M22" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="N22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -2457,50 +2363,47 @@
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-    </row>
-    <row r="23" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="8"/>
+    </row>
+    <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="E23" s="8" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" t="s">
-        <v>146</v>
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1</v>
       </c>
       <c r="I23" s="8">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="J23" s="8">
-        <v>1.07</v>
-      </c>
-      <c r="K23" s="8">
         <f t="shared" si="0"/>
         <v>1.07</v>
       </c>
+      <c r="K23" s="8">
+        <f>H23*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L23" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M23" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10.700000000000001</v>
       </c>
-      <c r="N23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
@@ -2520,50 +2423,47 @@
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="6"/>
-      <c r="AH23" s="6"/>
-    </row>
-    <row r="24" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="8">
-        <v>23</v>
+    </row>
+    <row r="24" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" t="s">
-        <v>147</v>
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1</v>
       </c>
       <c r="I24" s="8">
-        <v>1</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="J24" s="8">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="K24" s="8">
         <f t="shared" si="0"/>
         <v>0.53100000000000003</v>
       </c>
+      <c r="K24" s="8">
+        <f>H24*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L24" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M24" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.3100000000000005</v>
       </c>
-      <c r="N24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -2583,49 +2483,46 @@
       <c r="AE24" s="6"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-    </row>
-    <row r="25" spans="1:34" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="8">
-        <v>24</v>
+    </row>
+    <row r="25" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="16">
+        <v>57</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="15">
         <v>3983</v>
       </c>
+      <c r="E25" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F25" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" t="s">
-        <v>151</v>
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
       </c>
       <c r="I25" s="8">
-        <v>1</v>
+        <v>1.95</v>
       </c>
       <c r="J25" s="8">
-        <v>1.95</v>
-      </c>
-      <c r="K25" s="8">
         <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
+      <c r="K25" s="8">
+        <v>2</v>
+      </c>
       <c r="L25" s="8">
-        <v>2</v>
-      </c>
-      <c r="M25" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.9</v>
       </c>
-      <c r="N25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
@@ -2645,50 +2542,47 @@
       <c r="AE25" s="6"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
-    </row>
-    <row r="26" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="8">
-        <v>25</v>
+    </row>
+    <row r="26" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="16" t="s">
-        <v>152</v>
+        <v>65</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" t="s">
-        <v>153</v>
+        <v>15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
       </c>
       <c r="I26" s="8">
-        <v>1</v>
+        <v>1.64</v>
       </c>
       <c r="J26" s="8">
-        <v>1.64</v>
-      </c>
-      <c r="K26" s="8">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
+      <c r="K26" s="8">
+        <f>H26*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L26" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M26" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16.399999999999999</v>
       </c>
-      <c r="N26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
@@ -2708,50 +2602,47 @@
       <c r="AE26" s="6"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-    </row>
-    <row r="27" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="8">
-        <v>26</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="8"/>
+    </row>
+    <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="E27" s="8" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>155</v>
+        <v>145</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1</v>
       </c>
       <c r="I27" s="8">
-        <v>1</v>
+        <v>1.65</v>
       </c>
       <c r="J27" s="8">
-        <v>1.65</v>
-      </c>
-      <c r="K27" s="8">
         <f t="shared" si="0"/>
         <v>1.65</v>
       </c>
+      <c r="K27" s="8">
+        <f>H27*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L27" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M27" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
-      <c r="N27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -2771,50 +2662,47 @@
       <c r="AE27" s="6"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="6"/>
-      <c r="AH27" s="6"/>
-    </row>
-    <row r="28" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="8">
-        <v>27</v>
+    </row>
+    <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="16" t="s">
-        <v>156</v>
+        <v>62</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" t="s">
-        <v>157</v>
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>147</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
       </c>
       <c r="I28" s="8">
-        <v>1</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="J28" s="8">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="K28" s="8">
         <f t="shared" si="0"/>
         <v>0.54600000000000004</v>
       </c>
+      <c r="K28" s="8">
+        <f>H28*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L28" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M28" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.4600000000000009</v>
       </c>
-      <c r="N28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -2834,50 +2722,47 @@
       <c r="AE28" s="6"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="6"/>
-      <c r="AH28" s="6"/>
-    </row>
-    <row r="29" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="8">
-        <v>28</v>
+    </row>
+    <row r="29" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="16" t="s">
-        <v>158</v>
+        <v>64</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" t="s">
-        <v>159</v>
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
       </c>
       <c r="I29" s="8">
-        <v>1</v>
+        <v>0.871</v>
       </c>
       <c r="J29" s="8">
-        <v>0.871</v>
-      </c>
-      <c r="K29" s="8">
         <f t="shared" si="0"/>
         <v>0.871</v>
       </c>
+      <c r="K29" s="8">
+        <f>H29*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L29" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M29" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.7100000000000009</v>
       </c>
-      <c r="N29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
@@ -2897,50 +2782,47 @@
       <c r="AE29" s="6"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
-      <c r="AH29" s="6"/>
-    </row>
-    <row r="30" spans="1:34" ht="28" x14ac:dyDescent="0.15">
-      <c r="A30" s="8">
-        <v>29</v>
+    </row>
+    <row r="30" spans="1:33" ht="28" x14ac:dyDescent="0.15">
+      <c r="A30" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="16" t="s">
-        <v>160</v>
+        <v>68</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" t="s">
-        <v>161</v>
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
       </c>
       <c r="I30" s="8">
-        <v>1</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="J30" s="8">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="K30" s="8">
         <f t="shared" si="0"/>
         <v>0.27100000000000002</v>
       </c>
+      <c r="K30" s="8">
+        <f>H30*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L30" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M30" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.71</v>
       </c>
-      <c r="N30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
@@ -2960,50 +2842,47 @@
       <c r="AE30" s="6"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
-      <c r="AH30" s="6"/>
-    </row>
-    <row r="31" spans="1:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="A31" s="8">
-        <v>30</v>
+    </row>
+    <row r="31" spans="1:33" ht="14" x14ac:dyDescent="0.15">
+      <c r="A31" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="16" t="s">
-        <v>162</v>
+        <v>80</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" t="s">
-        <v>164</v>
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
       </c>
       <c r="I31" s="8">
-        <v>1</v>
+        <v>0.62</v>
       </c>
       <c r="J31" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="K31" s="8">
         <f t="shared" si="0"/>
         <v>0.62</v>
       </c>
+      <c r="K31" s="8">
+        <f>H31*$D$80</f>
+        <v>10</v>
+      </c>
       <c r="L31" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M31" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
-      <c r="N31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -3023,50 +2902,22 @@
       <c r="AE31" s="6"/>
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
-      <c r="AH31" s="6"/>
-    </row>
-    <row r="32" spans="1:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="A32" s="8">
-        <v>31</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" t="s">
-        <v>167</v>
-      </c>
-      <c r="I32" s="8">
-        <v>1</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0.28399999999999997</v>
-      </c>
-      <c r="K32" s="8">
-        <f t="shared" si="0"/>
-        <v>0.28399999999999997</v>
-      </c>
-      <c r="L32" s="8">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M32" s="8">
-        <f t="shared" si="2"/>
-        <v>2.84</v>
-      </c>
-      <c r="N32" s="12"/>
+    </row>
+    <row r="32" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A32" s="14"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
@@ -3086,25 +2937,33 @@
       <c r="AE32" s="6"/>
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
-      <c r="AH32" s="6"/>
-    </row>
-    <row r="33" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="8">
-        <v>32</v>
-      </c>
-      <c r="B33" s="15"/>
+    </row>
+    <row r="33" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="14"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="16"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="5"/>
+      <c r="J33" s="8">
+        <f>L33/K33</f>
+        <v>32.686999999999983</v>
+      </c>
+      <c r="K33" s="8">
+        <f>$D$80</f>
+        <v>10</v>
+      </c>
+      <c r="L33" s="8">
+        <f>SUM(L2:L32)</f>
+        <v>326.86999999999983</v>
+      </c>
+      <c r="M33" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
@@ -3124,16 +2983,13 @@
       <c r="AE33" s="6"/>
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-    </row>
-    <row r="34" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="8">
-        <v>33</v>
-      </c>
-      <c r="B34" s="15"/>
+    </row>
+    <row r="34" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A34" s="14"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="16"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -3141,13 +2997,8 @@
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="8">
-        <f>SUM(M2:M33)</f>
-        <v>327.31999999999982</v>
-      </c>
-      <c r="N34" s="27" t="s">
-        <v>168</v>
-      </c>
+      <c r="M34" s="5"/>
+      <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
@@ -3167,16 +3018,13 @@
       <c r="AE34" s="6"/>
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
-      <c r="AH34" s="6"/>
-    </row>
-    <row r="35" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="8">
-        <v>34</v>
-      </c>
-      <c r="B35" s="15"/>
+    </row>
+    <row r="35" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A35" s="14"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="16"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
@@ -3184,8 +3032,8 @@
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
@@ -3205,16 +3053,13 @@
       <c r="AE35" s="6"/>
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
-      <c r="AH35" s="6"/>
-    </row>
-    <row r="36" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="8">
-        <v>35</v>
-      </c>
-      <c r="B36" s="15"/>
+    </row>
+    <row r="36" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A36" s="14"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
@@ -3222,8 +3067,8 @@
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
@@ -3243,15 +3088,12 @@
       <c r="AE36" s="6"/>
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-    </row>
-    <row r="37" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="8">
-        <v>36</v>
-      </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+    </row>
+    <row r="37" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A37" s="14"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -3260,8 +3102,8 @@
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
@@ -3281,16 +3123,13 @@
       <c r="AE37" s="6"/>
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
-    </row>
-    <row r="38" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="8">
-        <v>37</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="16"/>
+    </row>
+    <row r="38" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="14"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -3298,8 +3137,8 @@
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
@@ -3319,16 +3158,13 @@
       <c r="AE38" s="6"/>
       <c r="AF38" s="6"/>
       <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
-    </row>
-    <row r="39" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="8">
-        <v>38</v>
-      </c>
-      <c r="B39" s="15"/>
+    </row>
+    <row r="39" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A39" s="14"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
@@ -3336,8 +3172,8 @@
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
@@ -3357,16 +3193,13 @@
       <c r="AE39" s="6"/>
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-    </row>
-    <row r="40" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A40" s="8">
-        <v>39</v>
-      </c>
-      <c r="B40" s="15"/>
+    </row>
+    <row r="40" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A40" s="14"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="16"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -3374,8 +3207,8 @@
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
@@ -3395,16 +3228,13 @@
       <c r="AE40" s="6"/>
       <c r="AF40" s="6"/>
       <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-    </row>
-    <row r="41" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="8">
-        <v>40</v>
-      </c>
-      <c r="B41" s="15"/>
+    </row>
+    <row r="41" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A41" s="14"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="16"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -3412,8 +3242,8 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
@@ -3433,16 +3263,13 @@
       <c r="AE41" s="6"/>
       <c r="AF41" s="6"/>
       <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
-    </row>
-    <row r="42" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A42" s="8">
-        <v>41</v>
-      </c>
-      <c r="B42" s="15"/>
+    </row>
+    <row r="42" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A42" s="14"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="16"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
@@ -3450,8 +3277,8 @@
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
@@ -3471,16 +3298,13 @@
       <c r="AE42" s="6"/>
       <c r="AF42" s="6"/>
       <c r="AG42" s="6"/>
-      <c r="AH42" s="6"/>
-    </row>
-    <row r="43" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="8">
-        <v>42</v>
-      </c>
-      <c r="B43" s="15"/>
+    </row>
+    <row r="43" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A43" s="14"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="16"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
@@ -3488,8 +3312,8 @@
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
@@ -3509,25 +3333,22 @@
       <c r="AE43" s="6"/>
       <c r="AF43" s="6"/>
       <c r="AG43" s="6"/>
-      <c r="AH43" s="6"/>
-    </row>
-    <row r="44" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="8">
-        <v>43</v>
-      </c>
-      <c r="B44" s="15"/>
+    </row>
+    <row r="44" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A44" s="14"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
@@ -3547,25 +3368,22 @@
       <c r="AE44" s="6"/>
       <c r="AF44" s="6"/>
       <c r="AG44" s="6"/>
-      <c r="AH44" s="6"/>
-    </row>
-    <row r="45" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="8">
-        <v>44</v>
-      </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="16"/>
+    </row>
+    <row r="45" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A45" s="14"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
+      <c r="G45" s="13"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
@@ -3585,25 +3403,22 @@
       <c r="AE45" s="6"/>
       <c r="AF45" s="6"/>
       <c r="AG45" s="6"/>
-      <c r="AH45" s="6"/>
-    </row>
-    <row r="46" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="8">
-        <v>45</v>
-      </c>
-      <c r="B46" s="15"/>
+    </row>
+    <row r="46" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A46" s="14"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="16"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="14"/>
+      <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="6"/>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
@@ -3623,16 +3438,13 @@
       <c r="AE46" s="6"/>
       <c r="AF46" s="6"/>
       <c r="AG46" s="6"/>
-      <c r="AH46" s="6"/>
-    </row>
-    <row r="47" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A47" s="8">
-        <v>46</v>
-      </c>
-      <c r="B47" s="15"/>
+    </row>
+    <row r="47" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A47" s="14"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="16"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -3640,8 +3452,8 @@
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
@@ -3661,16 +3473,13 @@
       <c r="AE47" s="6"/>
       <c r="AF47" s="6"/>
       <c r="AG47" s="6"/>
-      <c r="AH47" s="6"/>
-    </row>
-    <row r="48" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="8">
-        <v>47</v>
-      </c>
-      <c r="B48" s="15"/>
+    </row>
+    <row r="48" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A48" s="14"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="16"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -3678,8 +3487,8 @@
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="6"/>
@@ -3699,16 +3508,13 @@
       <c r="AE48" s="6"/>
       <c r="AF48" s="6"/>
       <c r="AG48" s="6"/>
-      <c r="AH48" s="6"/>
-    </row>
-    <row r="49" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="8">
-        <v>48</v>
-      </c>
-      <c r="B49" s="15"/>
+    </row>
+    <row r="49" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A49" s="14"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="16"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -3716,8 +3522,8 @@
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
@@ -3737,16 +3543,13 @@
       <c r="AE49" s="6"/>
       <c r="AF49" s="6"/>
       <c r="AG49" s="6"/>
-      <c r="AH49" s="6"/>
-    </row>
-    <row r="50" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="8">
-        <v>49</v>
-      </c>
-      <c r="B50" s="15"/>
+    </row>
+    <row r="50" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A50" s="14"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="16"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
@@ -3754,8 +3557,8 @@
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
@@ -3775,16 +3578,13 @@
       <c r="AE50" s="6"/>
       <c r="AF50" s="6"/>
       <c r="AG50" s="6"/>
-      <c r="AH50" s="6"/>
-    </row>
-    <row r="51" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="8">
-        <v>50</v>
-      </c>
-      <c r="B51" s="15"/>
+    </row>
+    <row r="51" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A51" s="14"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="16"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
@@ -3792,8 +3592,8 @@
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="6"/>
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
@@ -3813,16 +3613,13 @@
       <c r="AE51" s="6"/>
       <c r="AF51" s="6"/>
       <c r="AG51" s="6"/>
-      <c r="AH51" s="6"/>
-    </row>
-    <row r="52" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="8">
-        <v>51</v>
-      </c>
-      <c r="B52" s="15"/>
+    </row>
+    <row r="52" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A52" s="14"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="16"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
@@ -3830,8 +3627,8 @@
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="6"/>
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
@@ -3851,16 +3648,13 @@
       <c r="AE52" s="6"/>
       <c r="AF52" s="6"/>
       <c r="AG52" s="6"/>
-      <c r="AH52" s="6"/>
-    </row>
-    <row r="53" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="8">
-        <v>52</v>
-      </c>
-      <c r="B53" s="15"/>
+    </row>
+    <row r="53" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="14"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="16"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
@@ -3868,8 +3662,8 @@
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
@@ -3889,16 +3683,13 @@
       <c r="AE53" s="6"/>
       <c r="AF53" s="6"/>
       <c r="AG53" s="6"/>
-      <c r="AH53" s="6"/>
-    </row>
-    <row r="54" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="8">
-        <v>53</v>
-      </c>
-      <c r="B54" s="15"/>
+    </row>
+    <row r="54" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="14"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="16"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -3906,8 +3697,8 @@
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
@@ -3927,16 +3718,13 @@
       <c r="AE54" s="6"/>
       <c r="AF54" s="6"/>
       <c r="AG54" s="6"/>
-      <c r="AH54" s="6"/>
-    </row>
-    <row r="55" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="8">
-        <v>54</v>
-      </c>
-      <c r="B55" s="15"/>
+    </row>
+    <row r="55" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A55" s="14"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="16"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -3944,8 +3732,8 @@
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="6"/>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
@@ -3965,16 +3753,13 @@
       <c r="AE55" s="6"/>
       <c r="AF55" s="6"/>
       <c r="AG55" s="6"/>
-      <c r="AH55" s="6"/>
-    </row>
-    <row r="56" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="8">
-        <v>55</v>
-      </c>
-      <c r="B56" s="15"/>
+    </row>
+    <row r="56" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A56" s="14"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="16"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
@@ -3982,8 +3767,8 @@
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="6"/>
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="6"/>
@@ -4003,16 +3788,13 @@
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
       <c r="AG56" s="6"/>
-      <c r="AH56" s="6"/>
-    </row>
-    <row r="57" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="8">
-        <v>56</v>
-      </c>
-      <c r="B57" s="15"/>
+    </row>
+    <row r="57" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A57" s="14"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="16"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
@@ -4020,8 +3802,8 @@
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="6"/>
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
       <c r="Q57" s="6"/>
@@ -4041,16 +3823,13 @@
       <c r="AE57" s="6"/>
       <c r="AF57" s="6"/>
       <c r="AG57" s="6"/>
-      <c r="AH57" s="6"/>
-    </row>
-    <row r="58" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="8">
-        <v>57</v>
-      </c>
-      <c r="B58" s="15"/>
+    </row>
+    <row r="58" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A58" s="14"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="16"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
@@ -4058,8 +3837,8 @@
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="6"/>
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
@@ -4079,16 +3858,13 @@
       <c r="AE58" s="6"/>
       <c r="AF58" s="6"/>
       <c r="AG58" s="6"/>
-      <c r="AH58" s="6"/>
-    </row>
-    <row r="59" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="8">
-        <v>58</v>
-      </c>
-      <c r="B59" s="15"/>
+    </row>
+    <row r="59" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A59" s="14"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="16"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
@@ -4096,8 +3872,8 @@
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="6"/>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
@@ -4117,16 +3893,13 @@
       <c r="AE59" s="6"/>
       <c r="AF59" s="6"/>
       <c r="AG59" s="6"/>
-      <c r="AH59" s="6"/>
-    </row>
-    <row r="60" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A60" s="8">
-        <v>59</v>
-      </c>
-      <c r="B60" s="15"/>
+    </row>
+    <row r="60" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A60" s="14"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="16"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
@@ -4134,8 +3907,8 @@
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="6"/>
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
       <c r="Q60" s="6"/>
@@ -4155,16 +3928,13 @@
       <c r="AE60" s="6"/>
       <c r="AF60" s="6"/>
       <c r="AG60" s="6"/>
-      <c r="AH60" s="6"/>
-    </row>
-    <row r="61" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A61" s="8">
-        <v>60</v>
-      </c>
-      <c r="B61" s="15"/>
+    </row>
+    <row r="61" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A61" s="14"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="16"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
@@ -4172,8 +3942,8 @@
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="6"/>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
@@ -4193,16 +3963,13 @@
       <c r="AE61" s="6"/>
       <c r="AF61" s="6"/>
       <c r="AG61" s="6"/>
-      <c r="AH61" s="6"/>
-    </row>
-    <row r="62" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A62" s="8">
-        <v>61</v>
-      </c>
-      <c r="B62" s="15"/>
+    </row>
+    <row r="62" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A62" s="14"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="16"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
@@ -4210,8 +3977,8 @@
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="6"/>
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
       <c r="Q62" s="6"/>
@@ -4231,16 +3998,13 @@
       <c r="AE62" s="6"/>
       <c r="AF62" s="6"/>
       <c r="AG62" s="6"/>
-      <c r="AH62" s="6"/>
-    </row>
-    <row r="63" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A63" s="8">
-        <v>62</v>
-      </c>
-      <c r="B63" s="15"/>
+    </row>
+    <row r="63" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A63" s="14"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="16"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
@@ -4248,8 +4012,8 @@
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="6"/>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
       <c r="Q63" s="6"/>
@@ -4269,16 +4033,13 @@
       <c r="AE63" s="6"/>
       <c r="AF63" s="6"/>
       <c r="AG63" s="6"/>
-      <c r="AH63" s="6"/>
-    </row>
-    <row r="64" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A64" s="8">
-        <v>63</v>
-      </c>
-      <c r="B64" s="15"/>
+    </row>
+    <row r="64" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A64" s="14"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="16"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -4286,8 +4047,8 @@
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="6"/>
       <c r="O64" s="6"/>
       <c r="P64" s="6"/>
       <c r="Q64" s="6"/>
@@ -4307,16 +4068,13 @@
       <c r="AE64" s="6"/>
       <c r="AF64" s="6"/>
       <c r="AG64" s="6"/>
-      <c r="AH64" s="6"/>
-    </row>
-    <row r="65" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="8">
-        <v>64</v>
-      </c>
-      <c r="B65" s="15"/>
+    </row>
+    <row r="65" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A65" s="14"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="16"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
@@ -4324,8 +4082,8 @@
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="6"/>
       <c r="O65" s="6"/>
       <c r="P65" s="6"/>
       <c r="Q65" s="6"/>
@@ -4345,16 +4103,13 @@
       <c r="AE65" s="6"/>
       <c r="AF65" s="6"/>
       <c r="AG65" s="6"/>
-      <c r="AH65" s="6"/>
-    </row>
-    <row r="66" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A66" s="8">
-        <v>65</v>
-      </c>
-      <c r="B66" s="15"/>
+    </row>
+    <row r="66" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A66" s="14"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="16"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
@@ -4362,8 +4117,8 @@
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="6"/>
       <c r="O66" s="6"/>
       <c r="P66" s="6"/>
       <c r="Q66" s="6"/>
@@ -4383,16 +4138,13 @@
       <c r="AE66" s="6"/>
       <c r="AF66" s="6"/>
       <c r="AG66" s="6"/>
-      <c r="AH66" s="6"/>
-    </row>
-    <row r="67" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="8">
-        <v>66</v>
-      </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="16"/>
+    </row>
+    <row r="67" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A67" s="14"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
@@ -4400,8 +4152,8 @@
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
-      <c r="M67" s="8"/>
-      <c r="N67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="6"/>
       <c r="O67" s="6"/>
       <c r="P67" s="6"/>
       <c r="Q67" s="6"/>
@@ -4421,16 +4173,13 @@
       <c r="AE67" s="6"/>
       <c r="AF67" s="6"/>
       <c r="AG67" s="6"/>
-      <c r="AH67" s="6"/>
-    </row>
-    <row r="68" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="8">
-        <v>67</v>
-      </c>
-      <c r="B68" s="15"/>
+    </row>
+    <row r="68" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A68" s="14"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="16"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
@@ -4438,8 +4187,8 @@
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="6"/>
       <c r="O68" s="6"/>
       <c r="P68" s="6"/>
       <c r="Q68" s="6"/>
@@ -4459,16 +4208,13 @@
       <c r="AE68" s="6"/>
       <c r="AF68" s="6"/>
       <c r="AG68" s="6"/>
-      <c r="AH68" s="6"/>
-    </row>
-    <row r="69" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A69" s="8">
-        <v>68</v>
-      </c>
-      <c r="B69" s="15"/>
+    </row>
+    <row r="69" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A69" s="14"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="16"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
@@ -4476,8 +4222,8 @@
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="6"/>
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
       <c r="Q69" s="6"/>
@@ -4497,25 +4243,22 @@
       <c r="AE69" s="6"/>
       <c r="AF69" s="6"/>
       <c r="AG69" s="6"/>
-      <c r="AH69" s="6"/>
-    </row>
-    <row r="70" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="8">
-        <v>69</v>
-      </c>
-      <c r="B70" s="15"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="16"/>
+    </row>
+    <row r="70" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A70" s="14"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="8"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
+      <c r="G70" s="14"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="6"/>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
       <c r="Q70" s="6"/>
@@ -4535,25 +4278,22 @@
       <c r="AE70" s="6"/>
       <c r="AF70" s="6"/>
       <c r="AG70" s="6"/>
-      <c r="AH70" s="6"/>
-    </row>
-    <row r="71" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A71" s="8">
-        <v>70</v>
-      </c>
-      <c r="B71" s="15"/>
+    </row>
+    <row r="71" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="16"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="8"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
-      <c r="M71" s="8"/>
-      <c r="N71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="6"/>
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
       <c r="Q71" s="6"/>
@@ -4573,25 +4313,22 @@
       <c r="AE71" s="6"/>
       <c r="AF71" s="6"/>
       <c r="AG71" s="6"/>
-      <c r="AH71" s="6"/>
-    </row>
-    <row r="72" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A72" s="8">
-        <v>71</v>
-      </c>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="16"/>
+    </row>
+    <row r="72" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="8"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="16"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="5"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="6"/>
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
       <c r="Q72" s="6"/>
@@ -4611,25 +4348,22 @@
       <c r="AE72" s="6"/>
       <c r="AF72" s="6"/>
       <c r="AG72" s="6"/>
-      <c r="AH72" s="6"/>
-    </row>
-    <row r="73" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A73" s="8">
-        <v>72</v>
-      </c>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="16"/>
+    </row>
+    <row r="73" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A73" s="14"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="8"/>
       <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="16"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="8"/>
       <c r="I73" s="8"/>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="7"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="6"/>
       <c r="O73" s="6"/>
       <c r="P73" s="6"/>
       <c r="Q73" s="6"/>
@@ -4649,25 +4383,22 @@
       <c r="AE73" s="6"/>
       <c r="AF73" s="6"/>
       <c r="AG73" s="6"/>
-      <c r="AH73" s="6"/>
-    </row>
-    <row r="74" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A74" s="8">
-        <v>73</v>
-      </c>
-      <c r="B74" s="15"/>
+    </row>
+    <row r="74" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A74" s="14"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="16"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="8"/>
       <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="16"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
-      <c r="M74" s="8"/>
-      <c r="N74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="6"/>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
       <c r="Q74" s="6"/>
@@ -4687,25 +4418,21 @@
       <c r="AE74" s="6"/>
       <c r="AF74" s="6"/>
       <c r="AG74" s="6"/>
-      <c r="AH74" s="6"/>
-    </row>
-    <row r="75" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="8">
-        <v>74</v>
-      </c>
-      <c r="B75" s="15"/>
+    </row>
+    <row r="75" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A75" s="14"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="16"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="J75" s="12"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
-      <c r="M75" s="8"/>
-      <c r="N75" s="5"/>
+      <c r="M75" s="16"/>
+      <c r="N75" s="6"/>
       <c r="O75" s="6"/>
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
@@ -4725,22 +4452,21 @@
       <c r="AE75" s="6"/>
       <c r="AF75" s="6"/>
       <c r="AG75" s="6"/>
-      <c r="AH75" s="6"/>
-    </row>
-    <row r="76" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="8"/>
-      <c r="B76" s="15"/>
+    </row>
+    <row r="76" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A76" s="14"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="16"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="K76" s="13"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="8"/>
       <c r="L76" s="8"/>
-      <c r="M76" s="8"/>
-      <c r="N76" s="17"/>
+      <c r="M76" s="16"/>
+      <c r="N76" s="6"/>
       <c r="O76" s="6"/>
       <c r="P76" s="6"/>
       <c r="Q76" s="6"/>
@@ -4760,22 +4486,27 @@
       <c r="AE76" s="6"/>
       <c r="AF76" s="6"/>
       <c r="AG76" s="6"/>
-      <c r="AH76" s="6"/>
-    </row>
-    <row r="77" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A77" s="8"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="16"/>
+    </row>
+    <row r="77" spans="1:33" ht="28" x14ac:dyDescent="0.15">
+      <c r="A77" s="14"/>
+      <c r="B77" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="8"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
+      <c r="G77" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="K77" s="13"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
       <c r="L77" s="8"/>
-      <c r="M77" s="8"/>
-      <c r="N77" s="17"/>
+      <c r="M77" s="16"/>
+      <c r="N77" s="6"/>
       <c r="O77" s="6"/>
       <c r="P77" s="6"/>
       <c r="Q77" s="6"/>
@@ -4795,28 +4526,33 @@
       <c r="AE77" s="6"/>
       <c r="AF77" s="6"/>
       <c r="AG77" s="6"/>
-      <c r="AH77" s="6"/>
-    </row>
-    <row r="78" spans="1:34" ht="28" x14ac:dyDescent="0.15">
-      <c r="A78" s="8"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="18" t="s">
+    </row>
+    <row r="78" spans="1:33" ht="14" x14ac:dyDescent="0.15">
+      <c r="A78" s="14"/>
+      <c r="B78" s="18">
+        <f>SUM(J2:J74)</f>
+        <v>66.933999999999983</v>
+      </c>
+      <c r="C78" s="18"/>
+      <c r="D78" s="19">
+        <f>SUM(L2:L74)</f>
+        <v>653.73999999999967</v>
+      </c>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="G78" s="23">
+        <f>SUM(L2:L70)*1.3+L74</f>
+        <v>849.86199999999963</v>
+      </c>
+      <c r="H78" s="8"/>
       <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
-      <c r="M78" s="8"/>
-      <c r="N78" s="17"/>
+      <c r="M78" s="16"/>
+      <c r="N78" s="6"/>
       <c r="O78" s="6"/>
       <c r="P78" s="6"/>
       <c r="Q78" s="6"/>
@@ -4836,34 +4572,22 @@
       <c r="AE78" s="6"/>
       <c r="AF78" s="6"/>
       <c r="AG78" s="6"/>
-      <c r="AH78" s="6"/>
-    </row>
-    <row r="79" spans="1:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="A79" s="8"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="19">
-        <f>SUM(K2:K75)</f>
-        <v>34.291999999999994</v>
-      </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="20">
-        <f>SUM(M2:M75)</f>
-        <v>654.63999999999965</v>
-      </c>
+    </row>
+    <row r="79" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A79" s="14"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="8"/>
       <c r="F79" s="8"/>
-      <c r="G79" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H79" s="24">
-        <f>SUM(M2:M71)*1.3+M75</f>
-        <v>851.03199999999958</v>
-      </c>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
       <c r="I79" s="8"/>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
-      <c r="M79" s="8"/>
-      <c r="N79" s="17"/>
+      <c r="M79" s="16"/>
+      <c r="N79" s="6"/>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
@@ -4883,14 +4607,17 @@
       <c r="AE79" s="6"/>
       <c r="AF79" s="6"/>
       <c r="AG79" s="6"/>
-      <c r="AH79" s="6"/>
-    </row>
-    <row r="80" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A80" s="8"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="16"/>
+    </row>
+    <row r="80" spans="1:33" ht="14" x14ac:dyDescent="0.15">
+      <c r="A80" s="14"/>
+      <c r="B80" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="20"/>
+      <c r="D80" s="21">
+        <v>10</v>
+      </c>
+      <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
@@ -4898,8 +4625,8 @@
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="17"/>
+      <c r="M80" s="16"/>
+      <c r="N80" s="6"/>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
       <c r="Q80" s="6"/>
@@ -4919,18 +4646,17 @@
       <c r="AE80" s="6"/>
       <c r="AF80" s="6"/>
       <c r="AG80" s="6"/>
-      <c r="AH80" s="6"/>
-    </row>
-    <row r="81" spans="1:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="A81" s="8"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="21" t="s">
+    </row>
+    <row r="81" spans="1:33" ht="14" x14ac:dyDescent="0.15">
+      <c r="A81" s="14"/>
+      <c r="B81" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="21"/>
-      <c r="E81" s="22">
-        <v>10</v>
-      </c>
+      <c r="C81" s="20"/>
+      <c r="D81" s="21">
+        <v>2</v>
+      </c>
+      <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -4938,8 +4664,8 @@
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="17"/>
+      <c r="M81" s="16"/>
+      <c r="N81" s="6"/>
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
       <c r="Q81" s="6"/>
@@ -4959,18 +4685,13 @@
       <c r="AE81" s="6"/>
       <c r="AF81" s="6"/>
       <c r="AG81" s="6"/>
-      <c r="AH81" s="6"/>
-    </row>
-    <row r="82" spans="1:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="A82" s="8"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="21"/>
-      <c r="E82" s="22">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="82" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A82" s="14"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
@@ -4978,8 +4699,8 @@
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
-      <c r="M82" s="8"/>
-      <c r="N82" s="17"/>
+      <c r="M82" s="16"/>
+      <c r="N82" s="6"/>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
       <c r="Q82" s="6"/>
@@ -4999,14 +4720,13 @@
       <c r="AE82" s="6"/>
       <c r="AF82" s="6"/>
       <c r="AG82" s="6"/>
-      <c r="AH82" s="6"/>
-    </row>
-    <row r="83" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A83" s="8"/>
-      <c r="B83" s="15"/>
+    </row>
+    <row r="83" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A83" s="14"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="16"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="8"/>
       <c r="F83" s="8"/>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
@@ -5014,8 +4734,8 @@
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
-      <c r="M83" s="8"/>
-      <c r="N83" s="17"/>
+      <c r="M83" s="16"/>
+      <c r="N83" s="6"/>
       <c r="O83" s="6"/>
       <c r="P83" s="6"/>
       <c r="Q83" s="6"/>
@@ -5035,14 +4755,13 @@
       <c r="AE83" s="6"/>
       <c r="AF83" s="6"/>
       <c r="AG83" s="6"/>
-      <c r="AH83" s="6"/>
-    </row>
-    <row r="84" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A84" s="8"/>
-      <c r="B84" s="15"/>
+    </row>
+    <row r="84" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="14"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="16"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="8"/>
       <c r="F84" s="8"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
@@ -5050,8 +4769,8 @@
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
       <c r="L84" s="8"/>
-      <c r="M84" s="8"/>
-      <c r="N84" s="17"/>
+      <c r="M84" s="16"/>
+      <c r="N84" s="6"/>
       <c r="O84" s="6"/>
       <c r="P84" s="6"/>
       <c r="Q84" s="6"/>
@@ -5071,14 +4790,13 @@
       <c r="AE84" s="6"/>
       <c r="AF84" s="6"/>
       <c r="AG84" s="6"/>
-      <c r="AH84" s="6"/>
-    </row>
-    <row r="85" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A85" s="8"/>
-      <c r="B85" s="15"/>
+    </row>
+    <row r="85" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" s="14"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="16"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="8"/>
       <c r="F85" s="8"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
@@ -5086,8 +4804,8 @@
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
-      <c r="M85" s="8"/>
-      <c r="N85" s="17"/>
+      <c r="M85" s="16"/>
+      <c r="N85" s="6"/>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
       <c r="Q85" s="6"/>
@@ -5107,14 +4825,13 @@
       <c r="AE85" s="6"/>
       <c r="AF85" s="6"/>
       <c r="AG85" s="6"/>
-      <c r="AH85" s="6"/>
-    </row>
-    <row r="86" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="8"/>
-      <c r="B86" s="15"/>
+    </row>
+    <row r="86" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" s="14"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="16"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="8"/>
       <c r="F86" s="8"/>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
@@ -5122,8 +4839,8 @@
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
-      <c r="M86" s="8"/>
-      <c r="N86" s="17"/>
+      <c r="M86" s="16"/>
+      <c r="N86" s="6"/>
       <c r="O86" s="6"/>
       <c r="P86" s="6"/>
       <c r="Q86" s="6"/>
@@ -5143,14 +4860,13 @@
       <c r="AE86" s="6"/>
       <c r="AF86" s="6"/>
       <c r="AG86" s="6"/>
-      <c r="AH86" s="6"/>
-    </row>
-    <row r="87" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="8"/>
-      <c r="B87" s="15"/>
+    </row>
+    <row r="87" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="14"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="16"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="8"/>
       <c r="F87" s="8"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
@@ -5158,8 +4874,8 @@
       <c r="J87" s="8"/>
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
-      <c r="M87" s="8"/>
-      <c r="N87" s="17"/>
+      <c r="M87" s="16"/>
+      <c r="N87" s="6"/>
       <c r="O87" s="6"/>
       <c r="P87" s="6"/>
       <c r="Q87" s="6"/>
@@ -5179,14 +4895,13 @@
       <c r="AE87" s="6"/>
       <c r="AF87" s="6"/>
       <c r="AG87" s="6"/>
-      <c r="AH87" s="6"/>
-    </row>
-    <row r="88" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="8"/>
-      <c r="B88" s="15"/>
+    </row>
+    <row r="88" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="14"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="16"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="8"/>
       <c r="F88" s="8"/>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
@@ -5194,8 +4909,8 @@
       <c r="J88" s="8"/>
       <c r="K88" s="8"/>
       <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="17"/>
+      <c r="M88" s="16"/>
+      <c r="N88" s="6"/>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
       <c r="Q88" s="6"/>
@@ -5215,14 +4930,13 @@
       <c r="AE88" s="6"/>
       <c r="AF88" s="6"/>
       <c r="AG88" s="6"/>
-      <c r="AH88" s="6"/>
-    </row>
-    <row r="89" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A89" s="8"/>
-      <c r="B89" s="15"/>
+    </row>
+    <row r="89" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="14"/>
+      <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="16"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="8"/>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
@@ -5230,8 +4944,8 @@
       <c r="J89" s="8"/>
       <c r="K89" s="8"/>
       <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="17"/>
+      <c r="M89" s="16"/>
+      <c r="N89" s="6"/>
       <c r="O89" s="6"/>
       <c r="P89" s="6"/>
       <c r="Q89" s="6"/>
@@ -5251,14 +4965,13 @@
       <c r="AE89" s="6"/>
       <c r="AF89" s="6"/>
       <c r="AG89" s="6"/>
-      <c r="AH89" s="6"/>
-    </row>
-    <row r="90" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="8"/>
-      <c r="B90" s="15"/>
+    </row>
+    <row r="90" spans="1:33" ht="13" x14ac:dyDescent="0.15">
+      <c r="A90" s="14"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="16"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="8"/>
       <c r="F90" s="8"/>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
@@ -5266,8 +4979,8 @@
       <c r="J90" s="8"/>
       <c r="K90" s="8"/>
       <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="17"/>
+      <c r="M90" s="16"/>
+      <c r="N90" s="6"/>
       <c r="O90" s="6"/>
       <c r="P90" s="6"/>
       <c r="Q90" s="6"/>
@@ -5287,54 +5000,17 @@
       <c r="AE90" s="6"/>
       <c r="AF90" s="6"/>
       <c r="AG90" s="6"/>
-      <c r="AH90" s="6"/>
-    </row>
-    <row r="91" spans="1:34" ht="13" x14ac:dyDescent="0.15">
-      <c r="A91" s="8"/>
-      <c r="B91" s="15"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="16"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="6"/>
-      <c r="P91" s="6"/>
-      <c r="Q91" s="6"/>
-      <c r="R91" s="6"/>
-      <c r="S91" s="6"/>
-      <c r="T91" s="6"/>
-      <c r="U91" s="6"/>
-      <c r="V91" s="6"/>
-      <c r="W91" s="6"/>
-      <c r="X91" s="6"/>
-      <c r="Y91" s="6"/>
-      <c r="Z91" s="6"/>
-      <c r="AA91" s="6"/>
-      <c r="AB91" s="6"/>
-      <c r="AC91" s="6"/>
-      <c r="AD91" s="6"/>
-      <c r="AE91" s="6"/>
-      <c r="AF91" s="6"/>
-      <c r="AG91" s="6"/>
-      <c r="AH91" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N9" r:id="rId1" xr:uid="{F831D2CE-76B3-234D-BD4A-73DE1278DECE}"/>
-    <hyperlink ref="N7" r:id="rId2" xr:uid="{C1A1C035-444D-C24B-BD4D-07B2B871C297}"/>
-    <hyperlink ref="N6" r:id="rId3" xr:uid="{6418FC0B-65AD-3F44-970A-8D24F5A533DB}"/>
-    <hyperlink ref="N5" r:id="rId4" xr:uid="{724C573B-6956-E049-8084-7ACD180AA172}"/>
-    <hyperlink ref="N4" r:id="rId5" xr:uid="{EE29F280-58CE-6B44-9A14-8C690E6A3A1E}"/>
-    <hyperlink ref="N3" r:id="rId6" xr:uid="{F8DBF046-AB16-1548-973A-181D294B8B9E}"/>
-    <hyperlink ref="N2" r:id="rId7" xr:uid="{967611F7-C042-434C-B256-78FBC2F5B5A8}"/>
-    <hyperlink ref="N15" r:id="rId8" xr:uid="{54B9AE77-666B-C146-8A35-041EC866EAC7}"/>
+    <hyperlink ref="M10" r:id="rId1" xr:uid="{F831D2CE-76B3-234D-BD4A-73DE1278DECE}"/>
+    <hyperlink ref="M7" r:id="rId2" xr:uid="{C1A1C035-444D-C24B-BD4D-07B2B871C297}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{6418FC0B-65AD-3F44-970A-8D24F5A533DB}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{724C573B-6956-E049-8084-7ACD180AA172}"/>
+    <hyperlink ref="M4" r:id="rId5" xr:uid="{EE29F280-58CE-6B44-9A14-8C690E6A3A1E}"/>
+    <hyperlink ref="M3" r:id="rId6" xr:uid="{F8DBF046-AB16-1548-973A-181D294B8B9E}"/>
+    <hyperlink ref="M2" r:id="rId7" xr:uid="{967611F7-C042-434C-B256-78FBC2F5B5A8}"/>
+    <hyperlink ref="M15" r:id="rId8" xr:uid="{54B9AE77-666B-C146-8A35-041EC866EAC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>